<commit_message>
separated YOS into its own table. changed structure of ProgramStudents to have degree_completed and specific years
</commit_message>
<xml_diff>
--- a/dashboard/apps/excel_import/excel_files/test_excels/test_db3.xlsx
+++ b/dashboard/apps/excel_import/excel_files/test_excels/test_db3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="49">
   <si>
     <t xml:space="preserve">Encrypted Student No</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t xml:space="preserve">YOS 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00B197BA7753B1F2CFD57570245D62E5</t>
   </si>
 </sst>
 </file>
@@ -404,15 +407,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="15.4438775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,8 +1113,67 @@
         <v>33</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V12" s="3" t="n">
+        <v>63.67</v>
+      </c>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="36">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:K1"/>
@@ -1145,6 +1207,9 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="I12:K12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added tests for person changing file name from txt to xlsx and for a person doing the same subject twice in the same year
</commit_message>
<xml_diff>
--- a/dashboard/apps/excel_import/excel_files/test_excels/test_db3.xlsx
+++ b/dashboard/apps/excel_import/excel_files/test_excels/test_db3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="50">
   <si>
     <t xml:space="preserve">Encrypted Student No</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">00B197BA7753B1F2CFD57570245D62E5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00B197BA7753B1F2CFD57570245D62E8</t>
   </si>
 </sst>
 </file>
@@ -407,15 +410,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="15.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="16.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,8 +1175,134 @@
         <v>33</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V13" s="3" t="n">
+        <v>63.67</v>
+      </c>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q14" s="3" t="n">
+        <v>66</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V14" s="3" t="n">
+        <v>63.67</v>
+      </c>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="42">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:K1"/>
@@ -1210,6 +1339,12 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I14:K14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>